<commit_message>
Fixed layer bounds calculations.
</commit_message>
<xml_diff>
--- a/layer settings.xlsx
+++ b/layer settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mullsy/workspace/MullsyMaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32D710AD-550F-5343-ADF1-4AD9A8E36E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522F4F07-B26F-CF47-8B5E-18C8ED4E3B30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{CAB51283-BA90-A441-A352-DF7A37257213}"/>
+    <workbookView xWindow="33780" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{CAB51283-BA90-A441-A352-DF7A37257213}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>110</v>

</xml_diff>